<commit_message>
Minor UI Tweaks / Updated Script
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://entuedu-my.sharepoint.com/personal/irfansya002_e_ntu_edu_sg/Documents/Y1S2/IDP - IM2073/Android/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\School\Bahoot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31B6B029-9318-4F2C-BE01-09B159405A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E29437-9542-4CA7-B68A-C9ECE83BBAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{604BC9EA-757D-4B55-8E35-F133499EF34C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>setID</t>
   </si>
@@ -228,6 +228,27 @@
   </si>
   <si>
     <t>generatePdf</t>
+  </si>
+  <si>
+    <t>In which access should a constructor be defined, so that object of the class can be created in any function?</t>
+  </si>
+  <si>
+    <t>Any access specifier will work</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Protected</t>
+  </si>
+  <si>
+    <t>Which access specifier is usually used for data members of a class?</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -579,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FF8AB8-C22C-43C8-BA89-F4B1CB14D14F}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,25 +724,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="H5">
         <v>2</v>
@@ -729,28 +750,28 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="H6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -758,77 +779,77 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -836,48 +857,48 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="H11">
         <v>3</v>
@@ -885,28 +906,28 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12">
         <v>4</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -914,24 +935,76 @@
         <v>4</v>
       </c>
       <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
         <v>59</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D15" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
         <v>63</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F15" t="s">
         <v>61</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G15" t="s">
         <v>62</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>1</v>
       </c>
     </row>
@@ -942,6 +1015,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000A082714181D4D4A87FF3BB3021D1B0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fcdd1f49f7e62f86fa0f382379ecfa5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="edcfe5c4-b0dc-4e3f-83f8-1c0404b5d1f2" xmlns:ns4="d2731c71-a006-4f3f-805a-f475e549534d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d1bfb1da6b6fd8404e506991e037713" ns3:_="" ns4:_="">
     <xsd:import namespace="edcfe5c4-b0dc-4e3f-83f8-1c0404b5d1f2"/>
@@ -1156,15 +1238,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1174,6 +1247,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1B5954-E90A-4F58-9B21-1CEC7386E462}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9B85EBD-7071-445E-A2DF-9CDE00B322A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1188,14 +1269,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B1B5954-E90A-4F58-9B21-1CEC7386E462}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>